<commit_message>
Correction in experiment definition for SD-VBS
</commit_message>
<xml_diff>
--- a/experiment/xlsx/experiments_SD-VBS.xlsx
+++ b/experiment/xlsx/experiments_SD-VBS.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="111">
   <si>
     <t xml:space="preserve">experiment number</t>
   </si>
@@ -124,156 +124,31 @@
     <t xml:space="preserve">'111'</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">BENCH</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_DISPARITY</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">_CORES3_64MB_READATTACK1_DISPINPUT32</t>
-    </r>
+    <t xml:space="preserve">BENCH_DISPARITY_CORES3_64MB_READATTACK1_DISPINPUT32</t>
   </si>
   <si>
     <t xml:space="preserve">'1111'</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">BENCH</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_DISPARITY</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">_CORES4_64MB_READATTACK1_DISPINPUT32</t>
-    </r>
+    <t xml:space="preserve">BENCH_DISPARITY_CORES4_64MB_READATTACK1_DISPINPUT32</t>
   </si>
   <si>
     <t xml:space="preserve">'13'</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">BENCH</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_DISPARITY</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">_CORES2_64MB_READATTACK2_DISPINPUT32</t>
-    </r>
+    <t xml:space="preserve">BENCH_DISPARITY_CORES2_64MB_READATTACK2_DISPINPUT32</t>
   </si>
   <si>
     <t xml:space="preserve">'133'</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">BENCH</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_DISPARITY</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">_CORES3_64MB_READATTACK2_DISPINPUT32</t>
-    </r>
+    <t xml:space="preserve">BENCH_DISPARITY_CORES3_64MB_READATTACK2_DISPINPUT32</t>
   </si>
   <si>
     <t xml:space="preserve">'1333'</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">BENCH</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_DISPARITY</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">_CORES4_64MB_READATTACK2_DISPINPUT32</t>
-    </r>
+    <t xml:space="preserve">BENCH_DISPARITY_CORES4_64MB_READATTACK2_DISPINPUT32</t>
   </si>
   <si>
     <t xml:space="preserve">'12'</t>
@@ -285,1583 +160,199 @@
     <t xml:space="preserve">'122'</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">BENCH</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_DISPARITY</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">_CORES3_64MB_WRITEATTACK1_DISPINPUT32</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">BENCH</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_DISPARITY</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">_CORES4_64MB_WRITEATTACK1_DISPINPUT32</t>
-    </r>
+    <t xml:space="preserve">BENCH_DISPARITY_CORES3_64MB_WRITEATTACK1_DISPINPUT32</t>
   </si>
   <si>
     <t xml:space="preserve">'14'</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">BENCH</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_DISPARITY</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">_CORES2_64MB_WRITEATTACK2_DISPINPUT32</t>
-    </r>
+    <t xml:space="preserve">BENCH_DISPARITY_CORES2_64MB_WRITEATTACK2_DISPINPUT32</t>
   </si>
   <si>
     <t xml:space="preserve">'144'</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">BENCH</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_DISPARITY</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">_CORES3_64MB_WRITEATTACK2_DISPINPUT32</t>
-    </r>
+    <t xml:space="preserve">BENCH_DISPARITY_CORES3_64MB_WRITEATTACK2_DISPINPUT32</t>
   </si>
   <si>
     <t xml:space="preserve">'1444'</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">BENCH</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_DISPARITY</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">_CORES4_64MB_WRITEATTACK2_DISPINPUT32</t>
-    </r>
+    <t xml:space="preserve">BENCH_DISPARITY_CORES4_64MB_WRITEATTACK2_DISPINPUT32</t>
   </si>
   <si>
     <t xml:space="preserve">BENCH_DISPARITY_CORES2_64MB_READATTACK1_DISPINPUT64</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">BENCH</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_DISPARITY</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">_CORES3_64MB_READATTACK1_DISPINPUT64</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">BENCH</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_DISPARITY</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">_CORES4_64MB_READATTACK1_DISPINPUT64</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">BENCH</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_DISPARITY</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">_CORES2_64MB_READATTACK2_DISPINPUT64</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">BENCH</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_DISPARITY</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">_CORES3_64MB_READATTACK2_DISPINPUT64</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">BENCH</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_DISPARITY</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">_CORES4_64MB_READATTACK2_DISPINPUT64</t>
-    </r>
+    <t xml:space="preserve">BENCH_DISPARITY_CORES3_64MB_READATTACK1_DISPINPUT64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENCH_DISPARITY_CORES4_64MB_READATTACK1_DISPINPUT64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENCH_DISPARITY_CORES2_64MB_READATTACK2_DISPINPUT64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENCH_DISPARITY_CORES3_64MB_READATTACK2_DISPINPUT64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENCH_DISPARITY_CORES4_64MB_READATTACK2_DISPINPUT64</t>
   </si>
   <si>
     <t xml:space="preserve">BENCH_DISPARITY_CORES2_64MB_WRITEATTACK1_DISPINPUT64</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">BENCH</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_DISPARITY</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">_CORES3_64MB_WRITEATTACK1_DISPINPUT64</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">BENCH</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_DISPARITY</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">_CORES4_64MB_WRITEATTACK1_DISPINPUT64</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">BENCH</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_DISPARITY</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">_CORES2_64MB_WRITEATTACK2_DISPINPUT64</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">BENCH</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_DISPARITY</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">_CORES3_64MB_WRITEATTACK2_DISPINPUT64</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">BENCH</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_DISPARITY</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">_CORES4_64MB_WRITEATTACK2_DISPINPUT64</t>
-    </r>
+    <t xml:space="preserve">BENCH_DISPARITY_CORES3_64MB_WRITEATTACK1_DISPINPUT64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENCH_DISPARITY_CORES2_64MB_WRITEATTACK2_DISPINPUT64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENCH_DISPARITY_CORES3_64MB_WRITEATTACK2_DISPINPUT64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENCH_DISPARITY_CORES4_64MB_WRITEATTACK2_DISPINPUT64</t>
   </si>
   <si>
     <t xml:space="preserve">BENCH_DISPARITY_CORES2_64MB_READATTACK1_DISPINPUT96</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">BENCH</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_DISPARITY</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">_CORES3_64MB_READATTACK1_DISPINPUT96</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">BENCH</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_DISPARITY</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">_CORES4_64MB_READATTACK1_DISPINPUT96</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">BENCH</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_DISPARITY</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">_CORES2_64MB_READATTACK2_DISPINPUT96</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">BENCH</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_DISPARITY</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">_CORES3_64MB_READATTACK2_DISPINPUT96</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">BENCH</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_DISPARITY</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">_CORES4_64MB_READATTACK2_DISPINPUT96</t>
-    </r>
+    <t xml:space="preserve">BENCH_DISPARITY_CORES3_64MB_READATTACK1_DISPINPUT96</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENCH_DISPARITY_CORES4_64MB_READATTACK1_DISPINPUT96</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENCH_DISPARITY_CORES2_64MB_READATTACK2_DISPINPUT96</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENCH_DISPARITY_CORES3_64MB_READATTACK2_DISPINPUT96</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENCH_DISPARITY_CORES4_64MB_READATTACK2_DISPINPUT96</t>
   </si>
   <si>
     <t xml:space="preserve">BENCH_DISPARITY_CORES2_64MB_WRITEATTACK1_DISPINPUT96</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">BENCH</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_DISPARITY</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">_CORES3_64MB_WRITEATTACK1_DISPINPUT96</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">BENCH</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_DISPARITY</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">_CORES4_64MB_WRITEATTACK1_DISPINPUT96</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">BENCH</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_DISPARITY</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">_CORES2_64MB_WRITEATTACK2_DISPINPUT96</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">BENCH</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_DISPARITY</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">_CORES3_64MB_WRITEATTACK2_DISPINPUT96</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">BENCH</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_DISPARITY</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">_CORES4_64MB_WRITEATTACK2_DISPINPUT96</t>
-    </r>
+    <t xml:space="preserve">BENCH_DISPARITY_CORES3_64MB_WRITEATTACK1_DISPINPUT96</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENCH_DISPARITY_CORES4_64MB_WRITEATTACK1_DISPINPUT96</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENCH_DISPARITY_CORES2_64MB_WRITEATTACK2_DISPINPUT96</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENCH_DISPARITY_CORES3_64MB_WRITEATTACK2_DISPINPUT96</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENCH_DISPARITY_CORES4_64MB_WRITEATTACK2_DISPINPUT96</t>
   </si>
   <si>
     <t xml:space="preserve">BENCH_DISPARITY_CORES2_64MB_READATTACK1_DISPINPUT128</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">BENCH</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_DISPARITY</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">_CORES3_64MB_READATTACK1_DISPINPUT128</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">BENCH</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_DISPARITY</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">_CORES4_64MB_READATTACK1_DISPINPUT128</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">BENCH</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_DISPARITY</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">_CORES2_64MB_READATTACK2_DISPINPUT128</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">BENCH</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_DISPARITY</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">_CORES3_64MB_READATTACK2_DISPINPUT128</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">BENCH</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_DISPARITY</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">_CORES4_64MB_READATTACK2_DISPINPUT128</t>
-    </r>
+    <t xml:space="preserve">BENCH_DISPARITY_CORES3_64MB_READATTACK1_DISPINPUT128</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENCH_DISPARITY_CORES4_64MB_READATTACK1_DISPINPUT128</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENCH_DISPARITY_CORES2_64MB_READATTACK2_DISPINPUT128</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENCH_DISPARITY_CORES3_64MB_READATTACK2_DISPINPUT128</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENCH_DISPARITY_CORES4_64MB_READATTACK2_DISPINPUT128</t>
   </si>
   <si>
     <t xml:space="preserve">BENCH_DISPARITY_CORES2_64MB_WRITEATTACK1_DISPINPUT128</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">BENCH</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_DISPARITY</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">_CORES3_64MB_WRITEATTACK1_DISPINPUT128</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">BENCH</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_DISPARITY</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">_CORES4_64MB_WRITEATTACK1_DISPINPUT128</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">BENCH</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_DISPARITY</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">_CORES2_64MB_WRITEATTACK2_DISPINPUT128</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">BENCH</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_DISPARITY</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">_CORES3_64MB_WRITEATTACK2_DISPINPUT128</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">BENCH</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_DISPARITY</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">_CORES4_64MB_WRITEATTACK2_DISPINPUT128</t>
-    </r>
+    <t xml:space="preserve">BENCH_DISPARITY_CORES3_64MB_WRITEATTACK1_DISPINPUT128</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENCH_DISPARITY_CORES4_64MB_WRITEATTACK1_DISPINPUT128</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENCH_DISPARITY_CORES2_64MB_WRITEATTACK2_DISPINPUT128</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENCH_DISPARITY_CORES3_64MB_WRITEATTACK2_DISPINPUT128</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENCH_DISPARITY_CORES4_64MB_WRITEATTACK2_DISPINPUT128</t>
   </si>
   <si>
     <t xml:space="preserve">BENCH_DISPARITY_CORES2_64MB_READATTACK1_DISPINPUT160</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">BENCH</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_DISPARITY</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">_CORES3_64MB_READATTACK1_DISPINPUT160</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">BENCH</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_DISPARITY</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">_CORES4_64MB_READATTACK1_DISPINPUT160</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">BENCH</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_DISPARITY</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">_CORES2_64MB_READATTACK2_DISPINPUT160</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">BENCH</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_DISPARITY</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">_CORES3_64MB_READATTACK2_DISPINPUT160</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">BENCH</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_DISPARITY</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">_CORES4_64MB_READATTACK2_DISPINPUT160</t>
-    </r>
+    <t xml:space="preserve">BENCH_DISPARITY_CORES3_64MB_READATTACK1_DISPINPUT160</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENCH_DISPARITY_CORES4_64MB_READATTACK1_DISPINPUT160</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENCH_DISPARITY_CORES2_64MB_READATTACK2_DISPINPUT160</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENCH_DISPARITY_CORES3_64MB_READATTACK2_DISPINPUT160</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENCH_DISPARITY_CORES4_64MB_READATTACK2_DISPINPUT160</t>
   </si>
   <si>
     <t xml:space="preserve">BENCH_DISPARITY_CORES2_64MB_WRITEATTACK1_DISPINPUT160</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">BENCH</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_DISPARITY</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">_CORES3_64MB_WRITEATTACK1_DISPINPUT160</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">BENCH</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_DISPARITY</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">_CORES4_64MB_WRITEATTACK1_DISPINPUT160</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">BENCH</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_DISPARITY</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">_CORES2_64MB_WRITEATTACK2_DISPINPUT160</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">BENCH</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_DISPARITY</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">_CORES3_64MB_WRITEATTACK2_DISPINPUT160</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">BENCH</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_DISPARITY</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">_CORES4_64MB_WRITEATTACK2_DISPINPUT160</t>
-    </r>
+    <t xml:space="preserve">BENCH_DISPARITY_CORES3_64MB_WRITEATTACK1_DISPINPUT160</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENCH_DISPARITY_CORES4_64MB_WRITEATTACK1_DISPINPUT160</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENCH_DISPARITY_CORES2_64MB_WRITEATTACK2_DISPINPUT160</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENCH_DISPARITY_CORES3_64MB_WRITEATTACK2_DISPINPUT160</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENCH_DISPARITY_CORES4_64MB_WRITEATTACK2_DISPINPUT160</t>
   </si>
   <si>
     <t xml:space="preserve">BENCH_DISPARITY_CORES2_64MB_READATTACK1_DISPINPUT192</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">BENCH</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_DISPARITY</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">_CORES3_64MB_READATTACK1_DISPINPUT192</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">BENCH</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_DISPARITY</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">_CORES4_64MB_READATTACK1_DISPINPUT192</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">BENCH</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_DISPARITY</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">_CORES2_64MB_READATTACK2_DISPINPUT192</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">BENCH</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_DISPARITY</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">_CORES3_64MB_READATTACK2_DISPINPUT192</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">BENCH</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_DISPARITY</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">_CORES4_64MB_READATTACK2_DISPINPUT192</t>
-    </r>
+    <t xml:space="preserve">BENCH_DISPARITY_CORES3_64MB_READATTACK1_DISPINPUT192</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENCH_DISPARITY_CORES4_64MB_READATTACK1_DISPINPUT192</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENCH_DISPARITY_CORES2_64MB_READATTACK2_DISPINPUT192</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENCH_DISPARITY_CORES3_64MB_READATTACK2_DISPINPUT192</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENCH_DISPARITY_CORES4_64MB_READATTACK2_DISPINPUT192</t>
   </si>
   <si>
     <t xml:space="preserve">BENCH_DISPARITY_CORES2_64MB_WRITEATTACK1_DISPINPUT192</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">BENCH</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_DISPARITY</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">_CORES3_64MB_WRITEATTACK1_DISPINPUT192</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">BENCH</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_DISPARITY</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">_CORES4_64MB_WRITEATTACK1_DISPINPUT192</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">BENCH</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_DISPARITY</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">_CORES2_64MB_WRITEATTACK2_DISPINPUT192</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">BENCH</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_DISPARITY</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">_CORES3_64MB_WRITEATTACK2_DISPINPUT192</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">BENCH</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">_DISPARITY</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">_CORES4_64MB_WRITEATTACK2_DISPINPUT192</t>
-    </r>
+    <t xml:space="preserve">BENCH_DISPARITY_CORES3_64MB_WRITEATTACK1_DISPINPUT192</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENCH_DISPARITY_CORES2_64MB_WRITEATTACK2_DISPINPUT192</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENCH_DISPARITY_CORES3_64MB_WRITEATTACK2_DISPINPUT192</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENCH_DISPARITY_CORES4_64MB_WRITEATTACK2_DISPINPUT192</t>
   </si>
 </sst>
 </file>
@@ -1872,7 +363,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1900,11 +391,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1985,11 +471,11 @@
   </sheetPr>
   <dimension ref="A1:O82"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A50" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4:A82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.09375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.97"/>
@@ -2908,7 +1394,7 @@
         <v>1048576</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="J19" s="1" t="s">
         <v>18</v>
@@ -2938,29 +1424,29 @@
         <v>29</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E20" s="3" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F20" s="3" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G20" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H20" s="0" t="n">
+        <v>1048576</v>
+      </c>
+      <c r="I20" s="0" t="s">
         <v>48</v>
-      </c>
-      <c r="D20" s="3" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E20" s="3" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F20" s="3" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G20" s="3" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="H20" s="0" t="n">
-        <v>1048576</v>
-      </c>
-      <c r="I20" s="0" t="s">
-        <v>49</v>
       </c>
       <c r="J20" s="1" t="s">
         <v>18</v>
@@ -2986,29 +1472,29 @@
         <v>32</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E21" s="3" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F21" s="3" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G21" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H21" s="0" t="n">
+        <v>1048576</v>
+      </c>
+      <c r="I21" s="0" t="s">
         <v>50</v>
-      </c>
-      <c r="D21" s="3" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E21" s="3" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F21" s="3" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G21" s="3" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="H21" s="0" t="n">
-        <v>1048576</v>
-      </c>
-      <c r="I21" s="0" t="s">
-        <v>51</v>
       </c>
       <c r="J21" s="1" t="s">
         <v>18</v>
@@ -3036,29 +1522,29 @@
         <v>24</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D22" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E22" s="3" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F22" s="3" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G22" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H22" s="0" t="n">
+        <v>1048576</v>
+      </c>
+      <c r="I22" s="0" t="s">
         <v>52</v>
-      </c>
-      <c r="D22" s="3" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E22" s="3" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F22" s="3" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G22" s="3" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="H22" s="0" t="n">
-        <v>1048576</v>
-      </c>
-      <c r="I22" s="0" t="s">
-        <v>53</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>18</v>
@@ -3110,7 +1596,7 @@
         <v>1048576</v>
       </c>
       <c r="I23" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J23" s="1" t="s">
         <v>18</v>
@@ -3158,7 +1644,7 @@
         <v>1048576</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J24" s="1" t="s">
         <v>18</v>
@@ -3208,7 +1694,7 @@
         <v>1048576</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J25" s="1" t="s">
         <v>18</v>
@@ -3260,7 +1746,7 @@
         <v>1048576</v>
       </c>
       <c r="I26" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J26" s="1" t="s">
         <v>18</v>
@@ -3308,7 +1794,7 @@
         <v>1048576</v>
       </c>
       <c r="I27" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J27" s="1" t="s">
         <v>18</v>
@@ -3358,7 +1844,7 @@
         <v>1048576</v>
       </c>
       <c r="I28" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J28" s="1" t="s">
         <v>18</v>
@@ -3410,7 +1896,7 @@
         <v>1048576</v>
       </c>
       <c r="I29" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J29" s="1" t="s">
         <v>18</v>
@@ -3458,7 +1944,7 @@
         <v>1048576</v>
       </c>
       <c r="I30" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J30" s="1" t="s">
         <v>18</v>
@@ -3508,7 +1994,7 @@
         <v>1048576</v>
       </c>
       <c r="I31" s="0" t="s">
-        <v>62</v>
+        <v>27</v>
       </c>
       <c r="J31" s="1" t="s">
         <v>18</v>
@@ -3538,7 +2024,7 @@
         <v>29</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D32" s="3" t="n">
         <f aca="false">FALSE()</f>
@@ -3560,7 +2046,7 @@
         <v>1048576</v>
       </c>
       <c r="I32" s="0" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J32" s="1" t="s">
         <v>18</v>
@@ -3586,7 +2072,7 @@
         <v>32</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D33" s="3" t="n">
         <f aca="false">FALSE()</f>
@@ -3608,7 +2094,7 @@
         <v>1048576</v>
       </c>
       <c r="I33" s="0" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="J33" s="1" t="s">
         <v>18</v>
@@ -3636,7 +2122,7 @@
         <v>24</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D34" s="3" t="n">
         <f aca="false">FALSE()</f>
@@ -3658,7 +2144,7 @@
         <v>1048576</v>
       </c>
       <c r="I34" s="0" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J34" s="1" t="s">
         <v>18</v>
@@ -3710,7 +2196,7 @@
         <v>1048576</v>
       </c>
       <c r="I35" s="0" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J35" s="1" t="s">
         <v>18</v>
@@ -3758,7 +2244,7 @@
         <v>1048576</v>
       </c>
       <c r="I36" s="0" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="J36" s="1" t="s">
         <v>18</v>
@@ -3808,7 +2294,7 @@
         <v>1048576</v>
       </c>
       <c r="I37" s="0" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J37" s="1" t="s">
         <v>18</v>
@@ -3860,7 +2346,7 @@
         <v>1048576</v>
       </c>
       <c r="I38" s="0" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J38" s="1" t="s">
         <v>18</v>
@@ -3908,7 +2394,7 @@
         <v>1048576</v>
       </c>
       <c r="I39" s="0" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="J39" s="1" t="s">
         <v>18</v>
@@ -3958,7 +2444,7 @@
         <v>1048576</v>
       </c>
       <c r="I40" s="0" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="J40" s="1" t="s">
         <v>18</v>
@@ -4010,7 +2496,7 @@
         <v>1048576</v>
       </c>
       <c r="I41" s="0" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="J41" s="1" t="s">
         <v>18</v>
@@ -4058,7 +2544,7 @@
         <v>1048576</v>
       </c>
       <c r="I42" s="0" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J42" s="1" t="s">
         <v>18</v>
@@ -4108,7 +2594,7 @@
         <v>1048576</v>
       </c>
       <c r="I43" s="0" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J43" s="1" t="s">
         <v>18</v>
@@ -4138,7 +2624,7 @@
         <v>29</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D44" s="3" t="n">
         <f aca="false">FALSE()</f>
@@ -4160,7 +2646,7 @@
         <v>1048576</v>
       </c>
       <c r="I44" s="0" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J44" s="1" t="s">
         <v>18</v>
@@ -4186,7 +2672,7 @@
         <v>32</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D45" s="3" t="n">
         <f aca="false">FALSE()</f>
@@ -4208,7 +2694,7 @@
         <v>1048576</v>
       </c>
       <c r="I45" s="0" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="J45" s="1" t="s">
         <v>18</v>
@@ -4236,7 +2722,7 @@
         <v>24</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D46" s="3" t="n">
         <f aca="false">FALSE()</f>
@@ -4258,7 +2744,7 @@
         <v>1048576</v>
       </c>
       <c r="I46" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J46" s="1" t="s">
         <v>18</v>
@@ -4281,8 +2767,8 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="n">
-        <f aca="false">A34+1</f>
-        <v>34</v>
+        <f aca="false">A46+1</f>
+        <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>29</v>
@@ -4310,7 +2796,7 @@
         <v>1048576</v>
       </c>
       <c r="I47" s="0" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J47" s="1" t="s">
         <v>18</v>
@@ -4330,7 +2816,7 @@
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="n">
         <f aca="false">A47+1</f>
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>32</v>
@@ -4358,7 +2844,7 @@
         <v>1048576</v>
       </c>
       <c r="I48" s="0" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J48" s="1" t="s">
         <v>18</v>
@@ -4380,7 +2866,7 @@
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="n">
         <f aca="false">A48+1</f>
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>24</v>
@@ -4408,7 +2894,7 @@
         <v>1048576</v>
       </c>
       <c r="I49" s="0" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J49" s="1" t="s">
         <v>18</v>
@@ -4432,7 +2918,7 @@
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="n">
         <f aca="false">A49+1</f>
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>29</v>
@@ -4460,7 +2946,7 @@
         <v>1048576</v>
       </c>
       <c r="I50" s="0" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="J50" s="1" t="s">
         <v>18</v>
@@ -4480,7 +2966,7 @@
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="n">
         <f aca="false">A50+1</f>
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>32</v>
@@ -4508,7 +2994,7 @@
         <v>1048576</v>
       </c>
       <c r="I51" s="0" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J51" s="1" t="s">
         <v>18</v>
@@ -4530,7 +3016,7 @@
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="n">
         <f aca="false">A51+1</f>
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>24</v>
@@ -4558,7 +3044,7 @@
         <v>1048576</v>
       </c>
       <c r="I52" s="0" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="J52" s="1" t="s">
         <v>18</v>
@@ -4582,7 +3068,7 @@
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="n">
         <f aca="false">A52+1</f>
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>29</v>
@@ -4610,7 +3096,7 @@
         <v>1048576</v>
       </c>
       <c r="I53" s="0" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="J53" s="1" t="s">
         <v>18</v>
@@ -4630,7 +3116,7 @@
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="n">
         <f aca="false">A53+1</f>
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>32</v>
@@ -4658,7 +3144,7 @@
         <v>1048576</v>
       </c>
       <c r="I54" s="0" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J54" s="1" t="s">
         <v>18</v>
@@ -4680,7 +3166,7 @@
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="n">
         <f aca="false">A54+1</f>
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>24</v>
@@ -4708,7 +3194,7 @@
         <v>1048576</v>
       </c>
       <c r="I55" s="0" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J55" s="1" t="s">
         <v>18</v>
@@ -4732,13 +3218,13 @@
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="n">
         <f aca="false">A55+1</f>
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>29</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D56" s="3" t="n">
         <f aca="false">FALSE()</f>
@@ -4760,7 +3246,7 @@
         <v>1048576</v>
       </c>
       <c r="I56" s="0" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J56" s="1" t="s">
         <v>18</v>
@@ -4780,13 +3266,13 @@
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="n">
         <f aca="false">A56+1</f>
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D57" s="3" t="n">
         <f aca="false">FALSE()</f>
@@ -4808,7 +3294,7 @@
         <v>1048576</v>
       </c>
       <c r="I57" s="0" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="J57" s="1" t="s">
         <v>18</v>
@@ -4830,13 +3316,13 @@
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="n">
         <f aca="false">A57+1</f>
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D58" s="3" t="n">
         <f aca="false">FALSE()</f>
@@ -4858,7 +3344,7 @@
         <v>1048576</v>
       </c>
       <c r="I58" s="0" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J58" s="1" t="s">
         <v>18</v>
@@ -4881,8 +3367,8 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="n">
-        <f aca="false">A46+1</f>
-        <v>46</v>
+        <f aca="false">A58+1</f>
+        <v>58</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>29</v>
@@ -4910,7 +3396,7 @@
         <v>1048576</v>
       </c>
       <c r="I59" s="0" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J59" s="1" t="s">
         <v>18</v>
@@ -4930,7 +3416,7 @@
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="n">
         <f aca="false">A59+1</f>
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>32</v>
@@ -4958,7 +3444,7 @@
         <v>1048576</v>
       </c>
       <c r="I60" s="0" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J60" s="1" t="s">
         <v>18</v>
@@ -4980,7 +3466,7 @@
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="n">
         <f aca="false">A60+1</f>
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>24</v>
@@ -5008,7 +3494,7 @@
         <v>1048576</v>
       </c>
       <c r="I61" s="0" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="J61" s="1" t="s">
         <v>18</v>
@@ -5032,7 +3518,7 @@
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="n">
         <f aca="false">A61+1</f>
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>29</v>
@@ -5060,7 +3546,7 @@
         <v>1048576</v>
       </c>
       <c r="I62" s="0" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J62" s="1" t="s">
         <v>18</v>
@@ -5080,7 +3566,7 @@
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="n">
         <f aca="false">A62+1</f>
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>32</v>
@@ -5108,7 +3594,7 @@
         <v>1048576</v>
       </c>
       <c r="I63" s="0" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J63" s="1" t="s">
         <v>18</v>
@@ -5130,7 +3616,7 @@
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="n">
         <f aca="false">A63+1</f>
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>24</v>
@@ -5158,7 +3644,7 @@
         <v>1048576</v>
       </c>
       <c r="I64" s="0" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J64" s="1" t="s">
         <v>18</v>
@@ -5182,7 +3668,7 @@
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="n">
         <f aca="false">A64+1</f>
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>29</v>
@@ -5210,7 +3696,7 @@
         <v>1048576</v>
       </c>
       <c r="I65" s="0" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J65" s="1" t="s">
         <v>18</v>
@@ -5230,7 +3716,7 @@
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="n">
         <f aca="false">A65+1</f>
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>32</v>
@@ -5258,7 +3744,7 @@
         <v>1048576</v>
       </c>
       <c r="I66" s="0" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="J66" s="1" t="s">
         <v>18</v>
@@ -5280,7 +3766,7 @@
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="n">
         <f aca="false">A66+1</f>
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>24</v>
@@ -5308,7 +3794,7 @@
         <v>1048576</v>
       </c>
       <c r="I67" s="0" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="J67" s="1" t="s">
         <v>18</v>
@@ -5332,13 +3818,13 @@
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="n">
         <f aca="false">A67+1</f>
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>29</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D68" s="3" t="n">
         <f aca="false">FALSE()</f>
@@ -5360,7 +3846,7 @@
         <v>1048576</v>
       </c>
       <c r="I68" s="0" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="J68" s="1" t="s">
         <v>18</v>
@@ -5380,13 +3866,13 @@
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="n">
         <f aca="false">A68+1</f>
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D69" s="3" t="n">
         <f aca="false">FALSE()</f>
@@ -5408,7 +3894,7 @@
         <v>1048576</v>
       </c>
       <c r="I69" s="0" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J69" s="1" t="s">
         <v>18</v>
@@ -5430,13 +3916,13 @@
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="n">
         <f aca="false">A69+1</f>
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D70" s="3" t="n">
         <f aca="false">FALSE()</f>
@@ -5458,7 +3944,7 @@
         <v>1048576</v>
       </c>
       <c r="I70" s="0" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="J70" s="1" t="s">
         <v>18</v>
@@ -5481,8 +3967,8 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="n">
-        <f aca="false">A58+1</f>
-        <v>46</v>
+        <f aca="false">A70+1</f>
+        <v>70</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>29</v>
@@ -5510,7 +3996,7 @@
         <v>1048576</v>
       </c>
       <c r="I71" s="0" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J71" s="1" t="s">
         <v>18</v>
@@ -5530,7 +4016,7 @@
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="n">
         <f aca="false">A71+1</f>
-        <v>47</v>
+        <v>71</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>32</v>
@@ -5558,7 +4044,7 @@
         <v>1048576</v>
       </c>
       <c r="I72" s="0" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J72" s="1" t="s">
         <v>18</v>
@@ -5580,7 +4066,7 @@
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="n">
         <f aca="false">A72+1</f>
-        <v>48</v>
+        <v>72</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>24</v>
@@ -5608,7 +4094,7 @@
         <v>1048576</v>
       </c>
       <c r="I73" s="0" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J73" s="1" t="s">
         <v>18</v>
@@ -5632,7 +4118,7 @@
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="n">
         <f aca="false">A73+1</f>
-        <v>49</v>
+        <v>73</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>29</v>
@@ -5660,7 +4146,7 @@
         <v>1048576</v>
       </c>
       <c r="I74" s="0" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J74" s="1" t="s">
         <v>18</v>
@@ -5680,7 +4166,7 @@
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="n">
         <f aca="false">A74+1</f>
-        <v>50</v>
+        <v>74</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>32</v>
@@ -5708,7 +4194,7 @@
         <v>1048576</v>
       </c>
       <c r="I75" s="0" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="J75" s="1" t="s">
         <v>18</v>
@@ -5730,7 +4216,7 @@
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="n">
         <f aca="false">A75+1</f>
-        <v>51</v>
+        <v>75</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>24</v>
@@ -5758,7 +4244,7 @@
         <v>1048576</v>
       </c>
       <c r="I76" s="0" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="J76" s="1" t="s">
         <v>18</v>
@@ -5782,7 +4268,7 @@
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="n">
         <f aca="false">A76+1</f>
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>29</v>
@@ -5810,7 +4296,7 @@
         <v>1048576</v>
       </c>
       <c r="I77" s="0" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="J77" s="1" t="s">
         <v>18</v>
@@ -5830,7 +4316,7 @@
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="n">
         <f aca="false">A77+1</f>
-        <v>53</v>
+        <v>77</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>32</v>
@@ -5858,7 +4344,7 @@
         <v>1048576</v>
       </c>
       <c r="I78" s="0" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="J78" s="1" t="s">
         <v>18</v>
@@ -5880,7 +4366,7 @@
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="n">
         <f aca="false">A78+1</f>
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>24</v>
@@ -5908,7 +4394,7 @@
         <v>1048576</v>
       </c>
       <c r="I79" s="0" t="s">
-        <v>110</v>
+        <v>28</v>
       </c>
       <c r="J79" s="1" t="s">
         <v>18</v>
@@ -5932,13 +4418,13 @@
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="n">
         <f aca="false">A79+1</f>
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>29</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D80" s="3" t="n">
         <f aca="false">FALSE()</f>
@@ -5960,7 +4446,7 @@
         <v>1048576</v>
       </c>
       <c r="I80" s="0" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="J80" s="1" t="s">
         <v>18</v>
@@ -5980,13 +4466,13 @@
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="n">
         <f aca="false">A80+1</f>
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D81" s="3" t="n">
         <f aca="false">FALSE()</f>
@@ -6008,7 +4494,7 @@
         <v>1048576</v>
       </c>
       <c r="I81" s="0" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="J81" s="1" t="s">
         <v>18</v>
@@ -6030,13 +4516,13 @@
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="n">
         <f aca="false">A81+1</f>
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D82" s="3" t="n">
         <f aca="false">FALSE()</f>
@@ -6058,7 +4544,7 @@
         <v>1048576</v>
       </c>
       <c r="I82" s="0" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="J82" s="1" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
Added new benchmark: Mälardalen matrix multiplication
</commit_message>
<xml_diff>
--- a/experiment/xlsx/experiments_SD-VBS.xlsx
+++ b/experiment/xlsx/experiments_SD-VBS.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="118">
   <si>
     <t xml:space="preserve">experiment number</t>
   </si>
@@ -65,6 +65,9 @@
   </si>
   <si>
     <t xml:space="preserve">bsort inputsize</t>
+  </si>
+  <si>
+    <t xml:space="preserve">matmult inputsize</t>
   </si>
   <si>
     <t xml:space="preserve">tick rate hz</t>
@@ -513,10 +516,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:V82"/>
+  <dimension ref="A1:W82"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q2" activeCellId="0" sqref="Q2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.12109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -529,12 +532,13 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="10" style="0" width="12.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="17.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="14.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="15.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="2" width="14.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="18.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="3" width="18.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="19.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="20.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="16.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="15.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="2" width="14.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="18.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="3" width="18.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="19.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="20.95"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -589,29 +593,32 @@
       <c r="Q1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="R1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="S1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="6" t="s">
+      <c r="T1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="U1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="0"/>
+      <c r="V1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="0"/>
     </row>
     <row r="2" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D2" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -633,10 +640,10 @@
         <v>1048576</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -647,28 +654,31 @@
       <c r="O2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P2" s="8" t="n">
+      <c r="P2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="8" t="n">
         <v>18000</v>
       </c>
-      <c r="Q2" s="8" t="n">
+      <c r="R2" s="8" t="n">
         <v>676776</v>
       </c>
-      <c r="R2" s="9" t="n">
-        <f aca="false">U2/S2</f>
+      <c r="S2" s="9" t="n">
+        <f aca="false">V2/T2</f>
         <v>17731.1252172063</v>
       </c>
-      <c r="S2" s="8" t="n">
-        <f aca="false">Q2/10</f>
+      <c r="T2" s="8" t="n">
+        <f aca="false">R2/10</f>
         <v>67677.6</v>
       </c>
-      <c r="T2" s="3" t="n">
-        <f aca="false">Q2/(U2/P2)</f>
+      <c r="U2" s="3" t="n">
+        <f aca="false">R2/(V2/Q2)</f>
         <v>10.15164</v>
       </c>
-      <c r="U2" s="1" t="n">
+      <c r="V2" s="1" t="n">
         <v>1200000000</v>
       </c>
-      <c r="V2" s="0"/>
+      <c r="W2" s="0"/>
     </row>
     <row r="3" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
@@ -676,10 +686,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D3" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -701,10 +711,10 @@
         <v>1048576</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
@@ -715,28 +725,31 @@
       <c r="O3" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P3" s="8" t="n">
+      <c r="P3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="8" t="n">
         <v>5000</v>
       </c>
-      <c r="Q3" s="8" t="n">
+      <c r="R3" s="8" t="n">
         <v>2481557</v>
       </c>
-      <c r="R3" s="9" t="n">
-        <f aca="false">U3/S3</f>
+      <c r="S3" s="9" t="n">
+        <f aca="false">V3/T3</f>
         <v>4835.67373225761</v>
       </c>
-      <c r="S3" s="8" t="n">
-        <f aca="false">Q3/10</f>
+      <c r="T3" s="8" t="n">
+        <f aca="false">R3/10</f>
         <v>248155.7</v>
       </c>
-      <c r="T3" s="3" t="n">
-        <f aca="false">Q3/(U3/P3)</f>
+      <c r="U3" s="3" t="n">
+        <f aca="false">R3/(V3/Q3)</f>
         <v>10.3398208333333</v>
       </c>
-      <c r="U3" s="1" t="n">
+      <c r="V3" s="1" t="n">
         <v>1200000000</v>
       </c>
-      <c r="V3" s="0"/>
+      <c r="W3" s="0"/>
     </row>
     <row r="4" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
@@ -744,10 +757,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D4" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -769,10 +782,10 @@
         <v>1048576</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
@@ -783,28 +796,31 @@
       <c r="O4" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P4" s="8" t="n">
+      <c r="P4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="8" t="n">
         <v>2200</v>
       </c>
-      <c r="Q4" s="8" t="n">
+      <c r="R4" s="8" t="n">
         <v>5552704</v>
       </c>
-      <c r="R4" s="9" t="n">
-        <f aca="false">U4/S4</f>
+      <c r="S4" s="9" t="n">
+        <f aca="false">V4/T4</f>
         <v>2161.10925415797</v>
       </c>
-      <c r="S4" s="8" t="n">
-        <f aca="false">Q4/10</f>
+      <c r="T4" s="8" t="n">
+        <f aca="false">R4/10</f>
         <v>555270.4</v>
       </c>
-      <c r="T4" s="3" t="n">
-        <f aca="false">Q4/(U4/P4)</f>
+      <c r="U4" s="3" t="n">
+        <f aca="false">R4/(V4/Q4)</f>
         <v>10.1799573333333</v>
       </c>
-      <c r="U4" s="1" t="n">
+      <c r="V4" s="1" t="n">
         <v>1200000000</v>
       </c>
-      <c r="V4" s="0"/>
+      <c r="W4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
@@ -812,10 +828,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D5" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -837,10 +853,10 @@
         <v>1048576</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
@@ -851,25 +867,28 @@
       <c r="O5" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P5" s="8" t="n">
+      <c r="P5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="8" t="n">
         <v>1200</v>
       </c>
-      <c r="Q5" s="8" t="n">
+      <c r="R5" s="8" t="n">
         <v>10184913</v>
       </c>
-      <c r="R5" s="9" t="n">
-        <f aca="false">U5/S5</f>
+      <c r="S5" s="9" t="n">
+        <f aca="false">V5/T5</f>
         <v>1178.21330432572</v>
       </c>
-      <c r="S5" s="8" t="n">
-        <f aca="false">Q5/10</f>
+      <c r="T5" s="8" t="n">
+        <f aca="false">R5/10</f>
         <v>1018491.3</v>
       </c>
-      <c r="T5" s="3" t="n">
-        <f aca="false">Q5/(U5/P5)</f>
+      <c r="U5" s="3" t="n">
+        <f aca="false">R5/(V5/Q5)</f>
         <v>10.184913</v>
       </c>
-      <c r="U5" s="1" t="n">
+      <c r="V5" s="1" t="n">
         <v>1200000000</v>
       </c>
     </row>
@@ -879,10 +898,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D6" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -904,10 +923,10 @@
         <v>1048576</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
@@ -918,25 +937,28 @@
       <c r="O6" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P6" s="8" t="n">
+      <c r="P6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="8" t="n">
         <v>700</v>
       </c>
-      <c r="Q6" s="8" t="n">
+      <c r="R6" s="8" t="n">
         <v>17307105</v>
       </c>
-      <c r="R6" s="9" t="n">
-        <f aca="false">U6/S6</f>
+      <c r="S6" s="9" t="n">
+        <f aca="false">V6/T6</f>
         <v>693.356861242825</v>
       </c>
-      <c r="S6" s="8" t="n">
-        <f aca="false">Q6/10</f>
+      <c r="T6" s="8" t="n">
+        <f aca="false">R6/10</f>
         <v>1730710.5</v>
       </c>
-      <c r="T6" s="3" t="n">
-        <f aca="false">Q6/(U6/P6)</f>
+      <c r="U6" s="3" t="n">
+        <f aca="false">R6/(V6/Q6)</f>
         <v>10.09581125</v>
       </c>
-      <c r="U6" s="1" t="n">
+      <c r="V6" s="1" t="n">
         <v>1200000000</v>
       </c>
     </row>
@@ -946,10 +968,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D7" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -971,10 +993,10 @@
         <v>1048576</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
@@ -985,25 +1007,28 @@
       <c r="O7" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P7" s="8" t="n">
+      <c r="P7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="8" t="n">
         <v>500</v>
       </c>
-      <c r="Q7" s="8" t="n">
+      <c r="R7" s="8" t="n">
         <v>25423087</v>
       </c>
-      <c r="R7" s="9" t="n">
-        <f aca="false">U7/S7</f>
+      <c r="S7" s="9" t="n">
+        <f aca="false">V7/T7</f>
         <v>472.011915783477</v>
       </c>
-      <c r="S7" s="8" t="n">
-        <f aca="false">Q7/10</f>
+      <c r="T7" s="8" t="n">
+        <f aca="false">R7/10</f>
         <v>2542308.7</v>
       </c>
-      <c r="T7" s="3" t="n">
-        <f aca="false">Q7/(U7/P7)</f>
+      <c r="U7" s="3" t="n">
+        <f aca="false">R7/(V7/Q7)</f>
         <v>10.5929529166667</v>
       </c>
-      <c r="U7" s="1" t="n">
+      <c r="V7" s="1" t="n">
         <v>1200000000</v>
       </c>
     </row>
@@ -1013,10 +1038,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D8" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -1038,19 +1063,19 @@
         <v>1048576</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N8" s="0" t="n">
         <v>32</v>
@@ -1058,8 +1083,11 @@
       <c r="O8" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P8" s="0" t="n">
-        <f aca="false">P$2</f>
+      <c r="P8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="0" t="n">
+        <f aca="false">Q$2</f>
         <v>18000</v>
       </c>
     </row>
@@ -1069,10 +1097,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D9" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -1094,19 +1122,19 @@
         <v>1048576</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N9" s="0" t="n">
         <v>64</v>
@@ -1114,8 +1142,11 @@
       <c r="O9" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P9" s="0" t="n">
-        <f aca="false">P$3</f>
+      <c r="P9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="0" t="n">
+        <f aca="false">Q$3</f>
         <v>5000</v>
       </c>
     </row>
@@ -1125,10 +1156,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D10" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -1150,19 +1181,19 @@
         <v>1048576</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N10" s="0" t="n">
         <v>192</v>
@@ -1170,8 +1201,11 @@
       <c r="O10" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P10" s="0" t="n">
-        <f aca="false">P$7</f>
+      <c r="P10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="0" t="n">
+        <f aca="false">Q$7</f>
         <v>500</v>
       </c>
     </row>
@@ -1181,10 +1215,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D11" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -1206,13 +1240,13 @@
         <v>1048576</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
@@ -1222,8 +1256,11 @@
       <c r="O11" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P11" s="0" t="n">
-        <f aca="false">P$2</f>
+      <c r="P11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="0" t="n">
+        <f aca="false">Q$2</f>
         <v>18000</v>
       </c>
     </row>
@@ -1233,10 +1270,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D12" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -1258,16 +1295,16 @@
         <v>1048576</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M12" s="1"/>
       <c r="N12" s="0" t="n">
@@ -1276,8 +1313,11 @@
       <c r="O12" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P12" s="0" t="n">
-        <f aca="false">P$2</f>
+      <c r="P12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="0" t="n">
+        <f aca="false">Q$2</f>
         <v>18000</v>
       </c>
     </row>
@@ -1287,10 +1327,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D13" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -1312,19 +1352,19 @@
         <v>1048576</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N13" s="0" t="n">
         <v>32</v>
@@ -1332,8 +1372,11 @@
       <c r="O13" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P13" s="0" t="n">
-        <f aca="false">P$2</f>
+      <c r="P13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="0" t="n">
+        <f aca="false">Q$2</f>
         <v>18000</v>
       </c>
     </row>
@@ -1343,10 +1386,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D14" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -1368,13 +1411,13 @@
         <v>1048576</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
@@ -1384,8 +1427,11 @@
       <c r="O14" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P14" s="0" t="n">
-        <f aca="false">P$2</f>
+      <c r="P14" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="0" t="n">
+        <f aca="false">Q$2</f>
         <v>18000</v>
       </c>
     </row>
@@ -1395,10 +1441,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D15" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -1420,16 +1466,16 @@
         <v>1048576</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M15" s="1"/>
       <c r="N15" s="0" t="n">
@@ -1438,8 +1484,11 @@
       <c r="O15" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P15" s="0" t="n">
-        <f aca="false">P$2</f>
+      <c r="P15" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="0" t="n">
+        <f aca="false">Q$2</f>
         <v>18000</v>
       </c>
     </row>
@@ -1449,10 +1498,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D16" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -1474,19 +1523,19 @@
         <v>1048576</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N16" s="0" t="n">
         <v>32</v>
@@ -1494,8 +1543,11 @@
       <c r="O16" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P16" s="0" t="n">
-        <f aca="false">P$2</f>
+      <c r="P16" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="0" t="n">
+        <f aca="false">Q$2</f>
         <v>18000</v>
       </c>
     </row>
@@ -1505,10 +1557,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D17" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -1530,13 +1582,13 @@
         <v>1048576</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
@@ -1546,8 +1598,11 @@
       <c r="O17" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P17" s="0" t="n">
-        <f aca="false">P$2</f>
+      <c r="P17" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="0" t="n">
+        <f aca="false">Q$2</f>
         <v>18000</v>
       </c>
     </row>
@@ -1557,10 +1612,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D18" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -1582,16 +1637,16 @@
         <v>1048576</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M18" s="1"/>
       <c r="N18" s="0" t="n">
@@ -1600,8 +1655,11 @@
       <c r="O18" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P18" s="0" t="n">
-        <f aca="false">P$2</f>
+      <c r="P18" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="0" t="n">
+        <f aca="false">Q$2</f>
         <v>18000</v>
       </c>
     </row>
@@ -1611,10 +1669,10 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D19" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -1636,19 +1694,19 @@
         <v>1048576</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N19" s="0" t="n">
         <v>32</v>
@@ -1656,8 +1714,11 @@
       <c r="O19" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P19" s="0" t="n">
-        <f aca="false">P$2</f>
+      <c r="P19" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="0" t="n">
+        <f aca="false">Q$2</f>
         <v>18000</v>
       </c>
     </row>
@@ -1667,10 +1728,10 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D20" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -1692,13 +1753,13 @@
         <v>1048576</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
@@ -1708,8 +1769,11 @@
       <c r="O20" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P20" s="0" t="n">
-        <f aca="false">P$2</f>
+      <c r="P20" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="0" t="n">
+        <f aca="false">Q$2</f>
         <v>18000</v>
       </c>
     </row>
@@ -1719,10 +1783,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D21" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -1744,16 +1808,16 @@
         <v>1048576</v>
       </c>
       <c r="I21" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M21" s="1"/>
       <c r="N21" s="0" t="n">
@@ -1762,8 +1826,11 @@
       <c r="O21" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P21" s="0" t="n">
-        <f aca="false">P$2</f>
+      <c r="P21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="0" t="n">
+        <f aca="false">Q$2</f>
         <v>18000</v>
       </c>
     </row>
@@ -1773,10 +1840,10 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D22" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -1798,19 +1865,19 @@
         <v>1048576</v>
       </c>
       <c r="I22" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N22" s="0" t="n">
         <v>32</v>
@@ -1818,8 +1885,11 @@
       <c r="O22" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P22" s="0" t="n">
-        <f aca="false">P$2</f>
+      <c r="P22" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="0" t="n">
+        <f aca="false">Q$2</f>
         <v>18000</v>
       </c>
     </row>
@@ -1829,10 +1899,10 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D23" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -1854,13 +1924,13 @@
         <v>1048576</v>
       </c>
       <c r="I23" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
@@ -1870,8 +1940,11 @@
       <c r="O23" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P23" s="0" t="n">
-        <f aca="false">P$3</f>
+      <c r="P23" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="0" t="n">
+        <f aca="false">Q$3</f>
         <v>5000</v>
       </c>
     </row>
@@ -1881,10 +1954,10 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D24" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -1906,16 +1979,16 @@
         <v>1048576</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M24" s="1"/>
       <c r="N24" s="0" t="n">
@@ -1924,8 +1997,11 @@
       <c r="O24" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P24" s="0" t="n">
-        <f aca="false">P$3</f>
+      <c r="P24" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="0" t="n">
+        <f aca="false">Q$3</f>
         <v>5000</v>
       </c>
     </row>
@@ -1935,10 +2011,10 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D25" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -1960,19 +2036,19 @@
         <v>1048576</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N25" s="0" t="n">
         <v>64</v>
@@ -1980,8 +2056,11 @@
       <c r="O25" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P25" s="0" t="n">
-        <f aca="false">P$3</f>
+      <c r="P25" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="0" t="n">
+        <f aca="false">Q$3</f>
         <v>5000</v>
       </c>
     </row>
@@ -1991,10 +2070,10 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D26" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -2016,13 +2095,13 @@
         <v>1048576</v>
       </c>
       <c r="I26" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
@@ -2032,8 +2111,11 @@
       <c r="O26" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P26" s="0" t="n">
-        <f aca="false">P$3</f>
+      <c r="P26" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="0" t="n">
+        <f aca="false">Q$3</f>
         <v>5000</v>
       </c>
     </row>
@@ -2043,10 +2125,10 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D27" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -2068,16 +2150,16 @@
         <v>1048576</v>
       </c>
       <c r="I27" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M27" s="1"/>
       <c r="N27" s="0" t="n">
@@ -2086,8 +2168,11 @@
       <c r="O27" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P27" s="0" t="n">
-        <f aca="false">P$3</f>
+      <c r="P27" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="0" t="n">
+        <f aca="false">Q$3</f>
         <v>5000</v>
       </c>
     </row>
@@ -2097,10 +2182,10 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D28" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -2122,19 +2207,19 @@
         <v>1048576</v>
       </c>
       <c r="I28" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N28" s="0" t="n">
         <v>64</v>
@@ -2142,8 +2227,11 @@
       <c r="O28" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P28" s="0" t="n">
-        <f aca="false">P$3</f>
+      <c r="P28" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="0" t="n">
+        <f aca="false">Q$3</f>
         <v>5000</v>
       </c>
     </row>
@@ -2153,10 +2241,10 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D29" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -2178,13 +2266,13 @@
         <v>1048576</v>
       </c>
       <c r="I29" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
@@ -2194,8 +2282,11 @@
       <c r="O29" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P29" s="0" t="n">
-        <f aca="false">P$3</f>
+      <c r="P29" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="0" t="n">
+        <f aca="false">Q$3</f>
         <v>5000</v>
       </c>
     </row>
@@ -2205,10 +2296,10 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D30" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -2230,16 +2321,16 @@
         <v>1048576</v>
       </c>
       <c r="I30" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M30" s="1"/>
       <c r="N30" s="0" t="n">
@@ -2248,8 +2339,11 @@
       <c r="O30" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P30" s="0" t="n">
-        <f aca="false">P$3</f>
+      <c r="P30" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="0" t="n">
+        <f aca="false">Q$3</f>
         <v>5000</v>
       </c>
     </row>
@@ -2259,10 +2353,10 @@
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D31" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -2284,19 +2378,19 @@
         <v>1048576</v>
       </c>
       <c r="I31" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N31" s="0" t="n">
         <v>64</v>
@@ -2304,8 +2398,11 @@
       <c r="O31" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P31" s="0" t="n">
-        <f aca="false">P$3</f>
+      <c r="P31" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="0" t="n">
+        <f aca="false">Q$3</f>
         <v>5000</v>
       </c>
     </row>
@@ -2315,10 +2412,10 @@
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D32" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -2340,13 +2437,13 @@
         <v>1048576</v>
       </c>
       <c r="I32" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
@@ -2356,8 +2453,11 @@
       <c r="O32" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P32" s="0" t="n">
-        <f aca="false">P$3</f>
+      <c r="P32" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q32" s="0" t="n">
+        <f aca="false">Q$3</f>
         <v>5000</v>
       </c>
     </row>
@@ -2367,10 +2467,10 @@
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D33" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -2392,16 +2492,16 @@
         <v>1048576</v>
       </c>
       <c r="I33" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M33" s="1"/>
       <c r="N33" s="0" t="n">
@@ -2410,8 +2510,11 @@
       <c r="O33" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P33" s="0" t="n">
-        <f aca="false">P$3</f>
+      <c r="P33" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q33" s="0" t="n">
+        <f aca="false">Q$3</f>
         <v>5000</v>
       </c>
     </row>
@@ -2421,10 +2524,10 @@
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D34" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -2446,19 +2549,19 @@
         <v>1048576</v>
       </c>
       <c r="I34" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M34" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N34" s="0" t="n">
         <v>64</v>
@@ -2466,8 +2569,11 @@
       <c r="O34" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P34" s="0" t="n">
-        <f aca="false">P$3</f>
+      <c r="P34" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q34" s="0" t="n">
+        <f aca="false">Q$3</f>
         <v>5000</v>
       </c>
     </row>
@@ -2477,10 +2583,10 @@
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D35" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -2502,13 +2608,13 @@
         <v>1048576</v>
       </c>
       <c r="I35" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
@@ -2518,8 +2624,11 @@
       <c r="O35" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P35" s="0" t="n">
-        <f aca="false">P$4</f>
+      <c r="P35" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q35" s="0" t="n">
+        <f aca="false">Q$4</f>
         <v>2200</v>
       </c>
     </row>
@@ -2529,10 +2638,10 @@
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D36" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -2554,16 +2663,16 @@
         <v>1048576</v>
       </c>
       <c r="I36" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L36" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M36" s="1"/>
       <c r="N36" s="0" t="n">
@@ -2572,8 +2681,11 @@
       <c r="O36" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P36" s="0" t="n">
-        <f aca="false">P$4</f>
+      <c r="P36" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q36" s="0" t="n">
+        <f aca="false">Q$4</f>
         <v>2200</v>
       </c>
     </row>
@@ -2583,10 +2695,10 @@
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D37" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -2608,19 +2720,19 @@
         <v>1048576</v>
       </c>
       <c r="I37" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L37" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M37" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N37" s="0" t="n">
         <v>96</v>
@@ -2628,8 +2740,11 @@
       <c r="O37" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P37" s="0" t="n">
-        <f aca="false">P$4</f>
+      <c r="P37" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q37" s="0" t="n">
+        <f aca="false">Q$4</f>
         <v>2200</v>
       </c>
     </row>
@@ -2639,10 +2754,10 @@
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D38" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -2664,13 +2779,13 @@
         <v>1048576</v>
       </c>
       <c r="I38" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
@@ -2680,8 +2795,11 @@
       <c r="O38" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P38" s="0" t="n">
-        <f aca="false">P$4</f>
+      <c r="P38" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q38" s="0" t="n">
+        <f aca="false">Q$4</f>
         <v>2200</v>
       </c>
     </row>
@@ -2691,10 +2809,10 @@
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D39" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -2716,16 +2834,16 @@
         <v>1048576</v>
       </c>
       <c r="I39" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L39" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M39" s="1"/>
       <c r="N39" s="0" t="n">
@@ -2734,8 +2852,11 @@
       <c r="O39" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P39" s="0" t="n">
-        <f aca="false">P$4</f>
+      <c r="P39" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q39" s="0" t="n">
+        <f aca="false">Q$4</f>
         <v>2200</v>
       </c>
     </row>
@@ -2745,10 +2866,10 @@
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D40" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -2770,19 +2891,19 @@
         <v>1048576</v>
       </c>
       <c r="I40" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L40" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M40" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N40" s="0" t="n">
         <v>96</v>
@@ -2790,8 +2911,11 @@
       <c r="O40" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P40" s="0" t="n">
-        <f aca="false">P$4</f>
+      <c r="P40" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q40" s="0" t="n">
+        <f aca="false">Q$4</f>
         <v>2200</v>
       </c>
     </row>
@@ -2801,10 +2925,10 @@
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D41" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -2826,13 +2950,13 @@
         <v>1048576</v>
       </c>
       <c r="I41" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L41" s="1"/>
       <c r="M41" s="1"/>
@@ -2842,8 +2966,11 @@
       <c r="O41" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P41" s="0" t="n">
-        <f aca="false">P$4</f>
+      <c r="P41" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q41" s="0" t="n">
+        <f aca="false">Q$4</f>
         <v>2200</v>
       </c>
     </row>
@@ -2853,10 +2980,10 @@
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D42" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -2878,16 +3005,16 @@
         <v>1048576</v>
       </c>
       <c r="I42" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L42" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M42" s="1"/>
       <c r="N42" s="0" t="n">
@@ -2896,8 +3023,11 @@
       <c r="O42" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P42" s="0" t="n">
-        <f aca="false">P$4</f>
+      <c r="P42" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q42" s="0" t="n">
+        <f aca="false">Q$4</f>
         <v>2200</v>
       </c>
     </row>
@@ -2907,10 +3037,10 @@
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D43" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -2932,19 +3062,19 @@
         <v>1048576</v>
       </c>
       <c r="I43" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L43" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M43" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N43" s="0" t="n">
         <v>96</v>
@@ -2952,8 +3082,11 @@
       <c r="O43" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P43" s="0" t="n">
-        <f aca="false">P$4</f>
+      <c r="P43" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q43" s="0" t="n">
+        <f aca="false">Q$4</f>
         <v>2200</v>
       </c>
     </row>
@@ -2963,10 +3096,10 @@
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D44" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -2988,13 +3121,13 @@
         <v>1048576</v>
       </c>
       <c r="I44" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L44" s="1"/>
       <c r="M44" s="1"/>
@@ -3004,8 +3137,11 @@
       <c r="O44" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P44" s="0" t="n">
-        <f aca="false">P$4</f>
+      <c r="P44" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q44" s="0" t="n">
+        <f aca="false">Q$4</f>
         <v>2200</v>
       </c>
     </row>
@@ -3015,10 +3151,10 @@
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D45" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -3040,16 +3176,16 @@
         <v>1048576</v>
       </c>
       <c r="I45" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L45" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M45" s="1"/>
       <c r="N45" s="0" t="n">
@@ -3058,8 +3194,11 @@
       <c r="O45" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P45" s="0" t="n">
-        <f aca="false">P$4</f>
+      <c r="P45" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q45" s="0" t="n">
+        <f aca="false">Q$4</f>
         <v>2200</v>
       </c>
     </row>
@@ -3069,10 +3208,10 @@
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D46" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -3094,19 +3233,19 @@
         <v>1048576</v>
       </c>
       <c r="I46" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L46" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M46" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N46" s="0" t="n">
         <v>96</v>
@@ -3114,8 +3253,11 @@
       <c r="O46" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P46" s="0" t="n">
-        <f aca="false">P$4</f>
+      <c r="P46" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q46" s="0" t="n">
+        <f aca="false">Q$4</f>
         <v>2200</v>
       </c>
     </row>
@@ -3125,10 +3267,10 @@
         <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D47" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -3150,13 +3292,13 @@
         <v>1048576</v>
       </c>
       <c r="I47" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L47" s="1"/>
       <c r="M47" s="1"/>
@@ -3166,8 +3308,11 @@
       <c r="O47" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P47" s="0" t="n">
-        <f aca="false">P$5</f>
+      <c r="P47" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q47" s="0" t="n">
+        <f aca="false">Q$5</f>
         <v>1200</v>
       </c>
     </row>
@@ -3177,10 +3322,10 @@
         <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D48" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -3202,16 +3347,16 @@
         <v>1048576</v>
       </c>
       <c r="I48" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L48" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M48" s="1"/>
       <c r="N48" s="0" t="n">
@@ -3220,8 +3365,11 @@
       <c r="O48" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P48" s="0" t="n">
-        <f aca="false">P$5</f>
+      <c r="P48" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q48" s="0" t="n">
+        <f aca="false">Q$5</f>
         <v>1200</v>
       </c>
     </row>
@@ -3231,10 +3379,10 @@
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D49" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -3256,19 +3404,19 @@
         <v>1048576</v>
       </c>
       <c r="I49" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L49" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M49" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N49" s="0" t="n">
         <v>128</v>
@@ -3276,8 +3424,11 @@
       <c r="O49" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P49" s="0" t="n">
-        <f aca="false">P$5</f>
+      <c r="P49" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q49" s="0" t="n">
+        <f aca="false">Q$5</f>
         <v>1200</v>
       </c>
     </row>
@@ -3287,10 +3438,10 @@
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D50" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -3312,13 +3463,13 @@
         <v>1048576</v>
       </c>
       <c r="I50" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L50" s="1"/>
       <c r="M50" s="1"/>
@@ -3328,8 +3479,11 @@
       <c r="O50" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P50" s="0" t="n">
-        <f aca="false">P$5</f>
+      <c r="P50" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q50" s="0" t="n">
+        <f aca="false">Q$5</f>
         <v>1200</v>
       </c>
     </row>
@@ -3339,10 +3493,10 @@
         <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D51" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -3364,16 +3518,16 @@
         <v>1048576</v>
       </c>
       <c r="I51" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K51" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L51" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M51" s="1"/>
       <c r="N51" s="0" t="n">
@@ -3382,8 +3536,11 @@
       <c r="O51" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P51" s="0" t="n">
-        <f aca="false">P$5</f>
+      <c r="P51" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q51" s="0" t="n">
+        <f aca="false">Q$5</f>
         <v>1200</v>
       </c>
     </row>
@@ -3393,10 +3550,10 @@
         <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D52" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -3418,19 +3575,19 @@
         <v>1048576</v>
       </c>
       <c r="I52" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K52" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L52" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M52" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N52" s="0" t="n">
         <v>128</v>
@@ -3438,8 +3595,11 @@
       <c r="O52" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P52" s="0" t="n">
-        <f aca="false">P$5</f>
+      <c r="P52" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q52" s="0" t="n">
+        <f aca="false">Q$5</f>
         <v>1200</v>
       </c>
     </row>
@@ -3449,10 +3609,10 @@
         <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D53" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -3474,13 +3634,13 @@
         <v>1048576</v>
       </c>
       <c r="I53" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L53" s="1"/>
       <c r="M53" s="1"/>
@@ -3490,8 +3650,11 @@
       <c r="O53" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P53" s="0" t="n">
-        <f aca="false">P$5</f>
+      <c r="P53" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q53" s="0" t="n">
+        <f aca="false">Q$5</f>
         <v>1200</v>
       </c>
     </row>
@@ -3501,10 +3664,10 @@
         <v>53</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D54" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -3526,16 +3689,16 @@
         <v>1048576</v>
       </c>
       <c r="I54" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K54" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L54" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M54" s="1"/>
       <c r="N54" s="0" t="n">
@@ -3544,8 +3707,11 @@
       <c r="O54" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P54" s="0" t="n">
-        <f aca="false">P$5</f>
+      <c r="P54" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q54" s="0" t="n">
+        <f aca="false">Q$5</f>
         <v>1200</v>
       </c>
     </row>
@@ -3555,10 +3721,10 @@
         <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D55" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -3580,19 +3746,19 @@
         <v>1048576</v>
       </c>
       <c r="I55" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="J55" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K55" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L55" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M55" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N55" s="0" t="n">
         <v>128</v>
@@ -3600,8 +3766,11 @@
       <c r="O55" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P55" s="0" t="n">
-        <f aca="false">P$5</f>
+      <c r="P55" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q55" s="0" t="n">
+        <f aca="false">Q$5</f>
         <v>1200</v>
       </c>
     </row>
@@ -3611,10 +3780,10 @@
         <v>55</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D56" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -3636,13 +3805,13 @@
         <v>1048576</v>
       </c>
       <c r="I56" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="J56" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K56" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L56" s="1"/>
       <c r="M56" s="1"/>
@@ -3652,8 +3821,11 @@
       <c r="O56" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P56" s="0" t="n">
-        <f aca="false">P$5</f>
+      <c r="P56" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q56" s="0" t="n">
+        <f aca="false">Q$5</f>
         <v>1200</v>
       </c>
     </row>
@@ -3663,10 +3835,10 @@
         <v>56</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D57" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -3688,16 +3860,16 @@
         <v>1048576</v>
       </c>
       <c r="I57" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="J57" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K57" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L57" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M57" s="1"/>
       <c r="N57" s="0" t="n">
@@ -3706,8 +3878,11 @@
       <c r="O57" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P57" s="0" t="n">
-        <f aca="false">P$5</f>
+      <c r="P57" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q57" s="0" t="n">
+        <f aca="false">Q$5</f>
         <v>1200</v>
       </c>
     </row>
@@ -3717,10 +3892,10 @@
         <v>57</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D58" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -3742,19 +3917,19 @@
         <v>1048576</v>
       </c>
       <c r="I58" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="J58" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K58" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L58" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M58" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N58" s="0" t="n">
         <v>128</v>
@@ -3762,8 +3937,11 @@
       <c r="O58" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P58" s="0" t="n">
-        <f aca="false">P$5</f>
+      <c r="P58" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q58" s="0" t="n">
+        <f aca="false">Q$5</f>
         <v>1200</v>
       </c>
     </row>
@@ -3773,10 +3951,10 @@
         <v>58</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D59" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -3798,13 +3976,13 @@
         <v>1048576</v>
       </c>
       <c r="I59" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="J59" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K59" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L59" s="1"/>
       <c r="M59" s="1"/>
@@ -3814,8 +3992,11 @@
       <c r="O59" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P59" s="0" t="n">
-        <f aca="false">P$6</f>
+      <c r="P59" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q59" s="0" t="n">
+        <f aca="false">Q$6</f>
         <v>700</v>
       </c>
     </row>
@@ -3825,10 +4006,10 @@
         <v>59</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D60" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -3850,16 +4031,16 @@
         <v>1048576</v>
       </c>
       <c r="I60" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J60" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K60" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L60" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M60" s="1"/>
       <c r="N60" s="0" t="n">
@@ -3868,8 +4049,11 @@
       <c r="O60" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P60" s="0" t="n">
-        <f aca="false">P$6</f>
+      <c r="P60" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q60" s="0" t="n">
+        <f aca="false">Q$6</f>
         <v>700</v>
       </c>
     </row>
@@ -3879,10 +4063,10 @@
         <v>60</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D61" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -3904,19 +4088,19 @@
         <v>1048576</v>
       </c>
       <c r="I61" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="J61" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K61" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L61" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M61" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N61" s="0" t="n">
         <v>160</v>
@@ -3924,8 +4108,11 @@
       <c r="O61" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P61" s="0" t="n">
-        <f aca="false">P$6</f>
+      <c r="P61" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q61" s="0" t="n">
+        <f aca="false">Q$6</f>
         <v>700</v>
       </c>
     </row>
@@ -3935,10 +4122,10 @@
         <v>61</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D62" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -3960,13 +4147,13 @@
         <v>1048576</v>
       </c>
       <c r="I62" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="J62" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K62" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L62" s="1"/>
       <c r="M62" s="1"/>
@@ -3976,8 +4163,11 @@
       <c r="O62" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P62" s="0" t="n">
-        <f aca="false">P$6</f>
+      <c r="P62" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q62" s="0" t="n">
+        <f aca="false">Q$6</f>
         <v>700</v>
       </c>
     </row>
@@ -3987,10 +4177,10 @@
         <v>62</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D63" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -4012,16 +4202,16 @@
         <v>1048576</v>
       </c>
       <c r="I63" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="J63" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K63" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L63" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M63" s="1"/>
       <c r="N63" s="0" t="n">
@@ -4030,8 +4220,11 @@
       <c r="O63" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P63" s="0" t="n">
-        <f aca="false">P$6</f>
+      <c r="P63" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q63" s="0" t="n">
+        <f aca="false">Q$6</f>
         <v>700</v>
       </c>
     </row>
@@ -4041,10 +4234,10 @@
         <v>63</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D64" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -4066,19 +4259,19 @@
         <v>1048576</v>
       </c>
       <c r="I64" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="J64" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K64" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L64" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M64" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N64" s="0" t="n">
         <v>160</v>
@@ -4086,8 +4279,11 @@
       <c r="O64" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P64" s="0" t="n">
-        <f aca="false">P$6</f>
+      <c r="P64" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q64" s="0" t="n">
+        <f aca="false">Q$6</f>
         <v>700</v>
       </c>
     </row>
@@ -4097,10 +4293,10 @@
         <v>64</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D65" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -4122,13 +4318,13 @@
         <v>1048576</v>
       </c>
       <c r="I65" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J65" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K65" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L65" s="1"/>
       <c r="M65" s="1"/>
@@ -4138,8 +4334,11 @@
       <c r="O65" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P65" s="0" t="n">
-        <f aca="false">P$6</f>
+      <c r="P65" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q65" s="0" t="n">
+        <f aca="false">Q$6</f>
         <v>700</v>
       </c>
     </row>
@@ -4149,10 +4348,10 @@
         <v>65</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D66" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -4174,16 +4373,16 @@
         <v>1048576</v>
       </c>
       <c r="I66" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="J66" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K66" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L66" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M66" s="1"/>
       <c r="N66" s="0" t="n">
@@ -4192,8 +4391,11 @@
       <c r="O66" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P66" s="0" t="n">
-        <f aca="false">P$6</f>
+      <c r="P66" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q66" s="0" t="n">
+        <f aca="false">Q$6</f>
         <v>700</v>
       </c>
     </row>
@@ -4203,10 +4405,10 @@
         <v>66</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D67" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -4228,19 +4430,19 @@
         <v>1048576</v>
       </c>
       <c r="I67" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="J67" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K67" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L67" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M67" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N67" s="0" t="n">
         <v>160</v>
@@ -4248,8 +4450,11 @@
       <c r="O67" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P67" s="0" t="n">
-        <f aca="false">P$6</f>
+      <c r="P67" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q67" s="0" t="n">
+        <f aca="false">Q$6</f>
         <v>700</v>
       </c>
     </row>
@@ -4259,10 +4464,10 @@
         <v>67</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D68" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -4284,13 +4489,13 @@
         <v>1048576</v>
       </c>
       <c r="I68" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="J68" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K68" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L68" s="1"/>
       <c r="M68" s="1"/>
@@ -4300,8 +4505,11 @@
       <c r="O68" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P68" s="0" t="n">
-        <f aca="false">P$6</f>
+      <c r="P68" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q68" s="0" t="n">
+        <f aca="false">Q$6</f>
         <v>700</v>
       </c>
     </row>
@@ -4311,10 +4519,10 @@
         <v>68</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D69" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -4336,16 +4544,16 @@
         <v>1048576</v>
       </c>
       <c r="I69" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="J69" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K69" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L69" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M69" s="1"/>
       <c r="N69" s="0" t="n">
@@ -4354,8 +4562,11 @@
       <c r="O69" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P69" s="0" t="n">
-        <f aca="false">P$6</f>
+      <c r="P69" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q69" s="0" t="n">
+        <f aca="false">Q$6</f>
         <v>700</v>
       </c>
     </row>
@@ -4365,10 +4576,10 @@
         <v>69</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D70" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -4390,19 +4601,19 @@
         <v>1048576</v>
       </c>
       <c r="I70" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="J70" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K70" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L70" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M70" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N70" s="0" t="n">
         <v>160</v>
@@ -4410,8 +4621,11 @@
       <c r="O70" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P70" s="0" t="n">
-        <f aca="false">P$6</f>
+      <c r="P70" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q70" s="0" t="n">
+        <f aca="false">Q$6</f>
         <v>700</v>
       </c>
     </row>
@@ -4421,10 +4635,10 @@
         <v>70</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D71" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -4446,13 +4660,13 @@
         <v>1048576</v>
       </c>
       <c r="I71" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="J71" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K71" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L71" s="1"/>
       <c r="M71" s="1"/>
@@ -4462,8 +4676,11 @@
       <c r="O71" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P71" s="0" t="n">
-        <f aca="false">P$7</f>
+      <c r="P71" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q71" s="0" t="n">
+        <f aca="false">Q$7</f>
         <v>500</v>
       </c>
     </row>
@@ -4473,10 +4690,10 @@
         <v>71</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D72" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -4498,16 +4715,16 @@
         <v>1048576</v>
       </c>
       <c r="I72" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="J72" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K72" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L72" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M72" s="1"/>
       <c r="N72" s="0" t="n">
@@ -4516,8 +4733,11 @@
       <c r="O72" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P72" s="0" t="n">
-        <f aca="false">P$7</f>
+      <c r="P72" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q72" s="0" t="n">
+        <f aca="false">Q$7</f>
         <v>500</v>
       </c>
     </row>
@@ -4527,10 +4747,10 @@
         <v>72</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D73" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -4552,19 +4772,19 @@
         <v>1048576</v>
       </c>
       <c r="I73" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="J73" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K73" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L73" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M73" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N73" s="0" t="n">
         <v>192</v>
@@ -4572,8 +4792,11 @@
       <c r="O73" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P73" s="0" t="n">
-        <f aca="false">P$7</f>
+      <c r="P73" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q73" s="0" t="n">
+        <f aca="false">Q$7</f>
         <v>500</v>
       </c>
     </row>
@@ -4583,10 +4806,10 @@
         <v>73</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D74" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -4608,13 +4831,13 @@
         <v>1048576</v>
       </c>
       <c r="I74" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="J74" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K74" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L74" s="1"/>
       <c r="M74" s="1"/>
@@ -4624,8 +4847,11 @@
       <c r="O74" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P74" s="0" t="n">
-        <f aca="false">P$7</f>
+      <c r="P74" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q74" s="0" t="n">
+        <f aca="false">Q$7</f>
         <v>500</v>
       </c>
     </row>
@@ -4635,10 +4861,10 @@
         <v>74</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D75" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -4660,16 +4886,16 @@
         <v>1048576</v>
       </c>
       <c r="I75" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="J75" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K75" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L75" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M75" s="1"/>
       <c r="N75" s="0" t="n">
@@ -4678,8 +4904,11 @@
       <c r="O75" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P75" s="0" t="n">
-        <f aca="false">P$7</f>
+      <c r="P75" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q75" s="0" t="n">
+        <f aca="false">Q$7</f>
         <v>500</v>
       </c>
     </row>
@@ -4689,10 +4918,10 @@
         <v>75</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D76" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -4714,19 +4943,19 @@
         <v>1048576</v>
       </c>
       <c r="I76" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="J76" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K76" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L76" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M76" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N76" s="0" t="n">
         <v>192</v>
@@ -4734,8 +4963,11 @@
       <c r="O76" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P76" s="0" t="n">
-        <f aca="false">P$7</f>
+      <c r="P76" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q76" s="0" t="n">
+        <f aca="false">Q$7</f>
         <v>500</v>
       </c>
     </row>
@@ -4745,10 +4977,10 @@
         <v>76</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D77" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -4770,13 +5002,13 @@
         <v>1048576</v>
       </c>
       <c r="I77" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="J77" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K77" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L77" s="1"/>
       <c r="M77" s="1"/>
@@ -4786,8 +5018,11 @@
       <c r="O77" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P77" s="0" t="n">
-        <f aca="false">P$7</f>
+      <c r="P77" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q77" s="0" t="n">
+        <f aca="false">Q$7</f>
         <v>500</v>
       </c>
     </row>
@@ -4797,10 +5032,10 @@
         <v>77</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D78" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -4822,16 +5057,16 @@
         <v>1048576</v>
       </c>
       <c r="I78" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="J78" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K78" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L78" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M78" s="1"/>
       <c r="N78" s="0" t="n">
@@ -4840,8 +5075,11 @@
       <c r="O78" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P78" s="0" t="n">
-        <f aca="false">P$7</f>
+      <c r="P78" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q78" s="0" t="n">
+        <f aca="false">Q$7</f>
         <v>500</v>
       </c>
     </row>
@@ -4851,10 +5089,10 @@
         <v>78</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D79" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -4876,19 +5114,19 @@
         <v>1048576</v>
       </c>
       <c r="I79" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J79" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K79" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L79" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M79" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N79" s="0" t="n">
         <v>192</v>
@@ -4896,8 +5134,11 @@
       <c r="O79" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P79" s="0" t="n">
-        <f aca="false">P$7</f>
+      <c r="P79" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q79" s="0" t="n">
+        <f aca="false">Q$7</f>
         <v>500</v>
       </c>
     </row>
@@ -4907,10 +5148,10 @@
         <v>79</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D80" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -4932,13 +5173,13 @@
         <v>1048576</v>
       </c>
       <c r="I80" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="J80" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K80" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L80" s="1"/>
       <c r="M80" s="1"/>
@@ -4948,8 +5189,11 @@
       <c r="O80" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P80" s="0" t="n">
-        <f aca="false">P$7</f>
+      <c r="P80" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q80" s="0" t="n">
+        <f aca="false">Q$7</f>
         <v>500</v>
       </c>
     </row>
@@ -4959,10 +5203,10 @@
         <v>80</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D81" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -4984,16 +5228,16 @@
         <v>1048576</v>
       </c>
       <c r="I81" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="J81" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K81" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L81" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M81" s="1"/>
       <c r="N81" s="0" t="n">
@@ -5002,8 +5246,11 @@
       <c r="O81" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P81" s="0" t="n">
-        <f aca="false">P$7</f>
+      <c r="P81" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q81" s="0" t="n">
+        <f aca="false">Q$7</f>
         <v>500</v>
       </c>
     </row>
@@ -5013,10 +5260,10 @@
         <v>81</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D82" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -5038,19 +5285,19 @@
         <v>1048576</v>
       </c>
       <c r="I82" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="J82" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K82" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L82" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M82" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N82" s="0" t="n">
         <v>192</v>
@@ -5058,8 +5305,11 @@
       <c r="O82" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="P82" s="0" t="n">
-        <f aca="false">P$7</f>
+      <c r="P82" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q82" s="0" t="n">
+        <f aca="false">Q$7</f>
         <v>500</v>
       </c>
     </row>

</xml_diff>